<commit_message>
print Subworks in Excel
</commit_message>
<xml_diff>
--- a/ReportOut.xlsx
+++ b/ReportOut.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="46">
   <si>
     <t>Logo Arauco</t>
   </si>
@@ -110,13 +110,19 @@
     <t>Avance</t>
   </si>
   <si>
-    <t xml:space="preserve">Cambio de Caps (60cu) </t>
-  </si>
-  <si>
-    <t>Marcado de Caps</t>
+    <t xml:space="preserve">  8 Cambio de Caps (60cu) </t>
+  </si>
+  <si>
+    <t>Nueva67ffs8</t>
   </si>
   <si>
     <t>100%</t>
+  </si>
+  <si>
+    <t>Nueva90</t>
+  </si>
+  <si>
+    <t>Nueva7</t>
   </si>
   <si>
     <t>Observaciones</t>
@@ -654,7 +660,7 @@
   <dimension ref="A1:AMK45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1847,10 +1853,16 @@
     </row>
     <row r="21" spans="1:1025" customHeight="1" ht="12.8">
       <c r="B21" s="7"/>
+      <c r="C21" s="21" t="s">
+        <v>34</v>
+      </c>
       <c r="F21" s="8"/>
     </row>
     <row r="22" spans="1:1025" customHeight="1" ht="12.8">
       <c r="B22" s="7"/>
+      <c r="C22" s="21" t="s">
+        <v>35</v>
+      </c>
       <c r="F22" s="8"/>
     </row>
     <row r="23" spans="1:1025" customHeight="1" ht="12.8">
@@ -1900,39 +1912,39 @@
     <row r="34" spans="1:1025" customHeight="1" ht="12.8">
       <c r="B34" s="11"/>
       <c r="C34" s="12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D34" s="12"/>
       <c r="E34" s="12" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F34" s="15"/>
     </row>
     <row r="35" spans="1:1025" customHeight="1" ht="12.8">
       <c r="B35" s="17" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C35" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F35" s="8"/>
     </row>
     <row r="36" spans="1:1025" customHeight="1" ht="12.8">
       <c r="B36" s="17" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F36" s="8"/>
     </row>
     <row r="37" spans="1:1025" customHeight="1" ht="12.8">
       <c r="B37" s="17" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F37" s="8"/>
     </row>
     <row r="38" spans="1:1025" customHeight="1" ht="12.8">
       <c r="B38" s="13"/>
       <c r="C38" s="12" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D38" s="14"/>
       <c r="E38" s="14"/>
@@ -1940,13 +1952,13 @@
     </row>
     <row r="39" spans="1:1025" customHeight="1" ht="12.8">
       <c r="B39" s="10" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F39" s="8"/>
     </row>
@@ -1958,13 +1970,13 @@
     </row>
     <row r="41" spans="1:1025" customHeight="1" ht="12.8">
       <c r="B41" s="10" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F41" s="8"/>
     </row>

</xml_diff>

<commit_message>
convert dates and add bootstrap 3.3
</commit_message>
<xml_diff>
--- a/ReportOut.xlsx
+++ b/ReportOut.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="49">
   <si>
     <t>Logo Arauco</t>
   </si>
@@ -41,12 +41,18 @@
     <t>Supervisor turno día:</t>
   </si>
   <si>
+    <t>Mario Vidal</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ubicación del equipo: </t>
   </si>
   <si>
     <t>Supervisores turno noche:</t>
   </si>
   <si>
+    <t>Marcelino Vasquez</t>
+  </si>
+  <si>
     <t>Sistema bloqueado:</t>
   </si>
   <si>
@@ -56,9 +62,15 @@
     <t>Ito Planta Turno día:</t>
   </si>
   <si>
+    <t>Jaime Urra</t>
+  </si>
+  <si>
     <t>Ito Planta Turno noche:</t>
   </si>
   <si>
+    <t>Victor Cortes</t>
+  </si>
+  <si>
     <t>Horas Programadas</t>
   </si>
   <si>
@@ -74,9 +86,6 @@
     <t>Hora Inicio:</t>
   </si>
   <si>
-    <t>2017-04-16T00:32:13Z</t>
-  </si>
-  <si>
     <t>Término:</t>
   </si>
   <si>
@@ -114,6 +123,9 @@
   </si>
   <si>
     <t xml:space="preserve">Precalentamiento </t>
+  </si>
+  <si>
+    <t>16/04/2017 00:32:13</t>
   </si>
   <si>
     <t>100%</t>
@@ -1723,87 +1735,91 @@
       <c r="E9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="8"/>
+      <c r="F9" s="8" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="10" spans="1:1025" customHeight="1" ht="12.8">
       <c r="B10" s="9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="8"/>
+        <v>10</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="11" spans="1:1025" customHeight="1" ht="12.8">
       <c r="B11" s="10" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="8"/>
+        <v>14</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="12" spans="1:1025" customHeight="1" ht="12.8">
       <c r="B12" s="7"/>
       <c r="E12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" s="8"/>
+        <v>16</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="13" spans="1:1025" customHeight="1" ht="12.8">
       <c r="B13" s="11" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:1025" customHeight="1" ht="12.8">
       <c r="B14" s="10" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>19</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="F14" s="8"/>
     </row>
     <row r="15" spans="1:1025" customHeight="1" ht="12.8">
       <c r="B15" s="10" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>19</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="F15" s="8"/>
     </row>
     <row r="16" spans="1:1025" customHeight="1" ht="12.8">
       <c r="B16" s="10" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F16" s="8"/>
     </row>
     <row r="17" spans="1:1025" customHeight="1" ht="12.8">
       <c r="B17" s="13"/>
       <c r="C17" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D17" s="14"/>
       <c r="E17" s="14"/>
@@ -1811,49 +1827,57 @@
     </row>
     <row r="18" spans="1:1025" customHeight="1" ht="12.8">
       <c r="B18" s="10" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:1025" customHeight="1" ht="12.8">
       <c r="B19" s="7"/>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F19" s="8"/>
     </row>
     <row r="20" spans="1:1025" customHeight="1" ht="12.8">
       <c r="B20" s="7"/>
       <c r="C20" s="21" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D20" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="E20" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:1025" customHeight="1" ht="12.8">
       <c r="B21" s="7"/>
       <c r="C21" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="F21" s="8"/>
+        <v>38</v>
+      </c>
+      <c r="D21" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" t="s">
+        <v>36</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="22" spans="1:1025" customHeight="1" ht="12.8">
       <c r="B22" s="7"/>
@@ -1906,39 +1930,39 @@
     <row r="34" spans="1:1025" customHeight="1" ht="12.8">
       <c r="B34" s="11"/>
       <c r="C34" s="12" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D34" s="12"/>
       <c r="E34" s="12" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="F34" s="15"/>
     </row>
     <row r="35" spans="1:1025" customHeight="1" ht="12.8">
       <c r="B35" s="17" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C35" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F35" s="8"/>
     </row>
     <row r="36" spans="1:1025" customHeight="1" ht="12.8">
       <c r="B36" s="17" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="F36" s="8"/>
     </row>
     <row r="37" spans="1:1025" customHeight="1" ht="12.8">
       <c r="B37" s="17" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F37" s="8"/>
     </row>
     <row r="38" spans="1:1025" customHeight="1" ht="12.8">
       <c r="B38" s="13"/>
       <c r="C38" s="12" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D38" s="14"/>
       <c r="E38" s="14"/>
@@ -1946,13 +1970,13 @@
     </row>
     <row r="39" spans="1:1025" customHeight="1" ht="12.8">
       <c r="B39" s="10" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F39" s="8"/>
     </row>
@@ -1964,13 +1988,13 @@
     </row>
     <row r="41" spans="1:1025" customHeight="1" ht="12.8">
       <c r="B41" s="10" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F41" s="8"/>
     </row>

</xml_diff>

<commit_message>
add autentificaction user, no protecting route
</commit_message>
<xml_diff>
--- a/ReportOut.xlsx
+++ b/ReportOut.xlsx
@@ -151,7 +151,7 @@
     <t>60%</t>
   </si>
   <si>
-    <t>Cambio de caps 7</t>
+    <t>Marcado de Caps 2.9</t>
   </si>
   <si>
     <t>PARA DETALLES VER EN ESQUEMAS PROXIMA PAGINA</t>
@@ -25310,7 +25310,7 @@
       <c r="C24" s="46"/>
       <c r="D24" s="41"/>
       <c r="E24" s="41" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F24" s="41"/>
       <c r="G24" s="41"/>
@@ -25395,9 +25395,7 @@
       <c r="B25" s="45"/>
       <c r="C25" s="46"/>
       <c r="D25" s="41"/>
-      <c r="E25" s="41" t="s">
-        <v>37</v>
-      </c>
+      <c r="E25" s="41"/>
       <c r="F25" s="41"/>
       <c r="G25" s="41"/>
       <c r="H25" s="41"/>
@@ -25420,25 +25418,19 @@
       <c r="Y25" s="41"/>
       <c r="Z25" s="41"/>
       <c r="AA25" s="41"/>
-      <c r="AB25" s="49" t="s">
-        <v>38</v>
-      </c>
+      <c r="AB25" s="49"/>
       <c r="AC25" s="49"/>
       <c r="AD25" s="49"/>
       <c r="AE25" s="49"/>
       <c r="AF25" s="49"/>
       <c r="AG25" s="49"/>
-      <c r="AH25" s="49" t="s">
-        <v>39</v>
-      </c>
+      <c r="AH25" s="49"/>
       <c r="AI25" s="49"/>
       <c r="AJ25" s="49"/>
       <c r="AK25" s="49"/>
       <c r="AL25" s="49"/>
       <c r="AM25" s="49"/>
-      <c r="AN25" s="44" t="s">
-        <v>40</v>
-      </c>
+      <c r="AN25" s="44"/>
       <c r="AO25" s="44"/>
       <c r="AP25" s="44"/>
       <c r="AQ25" s="44"/>
@@ -25481,9 +25473,7 @@
       <c r="B26" s="45"/>
       <c r="C26" s="46"/>
       <c r="D26" s="41"/>
-      <c r="E26" s="41" t="s">
-        <v>37</v>
-      </c>
+      <c r="E26" s="41"/>
       <c r="F26" s="41"/>
       <c r="G26" s="41"/>
       <c r="H26" s="41"/>
@@ -25506,25 +25496,19 @@
       <c r="Y26" s="41"/>
       <c r="Z26" s="41"/>
       <c r="AA26" s="41"/>
-      <c r="AB26" s="47" t="s">
-        <v>38</v>
-      </c>
+      <c r="AB26" s="47"/>
       <c r="AC26" s="47"/>
       <c r="AD26" s="47"/>
       <c r="AE26" s="47"/>
       <c r="AF26" s="47"/>
       <c r="AG26" s="47"/>
-      <c r="AH26" s="47" t="s">
-        <v>39</v>
-      </c>
+      <c r="AH26" s="47"/>
       <c r="AI26" s="47"/>
       <c r="AJ26" s="47"/>
       <c r="AK26" s="47"/>
       <c r="AL26" s="47"/>
       <c r="AM26" s="47"/>
-      <c r="AN26" s="48" t="s">
-        <v>40</v>
-      </c>
+      <c r="AN26" s="48"/>
       <c r="AO26" s="48"/>
       <c r="AP26" s="48"/>
       <c r="AQ26" s="48"/>
@@ -26514,9 +26498,7 @@
       <c r="A27" s="11"/>
       <c r="B27" s="45"/>
       <c r="C27" s="41"/>
-      <c r="D27" s="41" t="s">
-        <v>41</v>
-      </c>
+      <c r="D27" s="41"/>
       <c r="E27" s="41"/>
       <c r="F27" s="41"/>
       <c r="G27" s="41"/>
@@ -27543,9 +27525,7 @@
       <c r="B28" s="45"/>
       <c r="C28" s="46"/>
       <c r="D28" s="41"/>
-      <c r="E28" s="41" t="s">
-        <v>37</v>
-      </c>
+      <c r="E28" s="41"/>
       <c r="F28" s="41"/>
       <c r="G28" s="41"/>
       <c r="H28" s="41"/>
@@ -27568,25 +27548,19 @@
       <c r="Y28" s="41"/>
       <c r="Z28" s="41"/>
       <c r="AA28" s="41"/>
-      <c r="AB28" s="47" t="s">
-        <v>38</v>
-      </c>
+      <c r="AB28" s="47"/>
       <c r="AC28" s="47"/>
       <c r="AD28" s="47"/>
       <c r="AE28" s="47"/>
       <c r="AF28" s="47"/>
       <c r="AG28" s="47"/>
-      <c r="AH28" s="47" t="s">
-        <v>39</v>
-      </c>
+      <c r="AH28" s="47"/>
       <c r="AI28" s="47"/>
       <c r="AJ28" s="47"/>
       <c r="AK28" s="47"/>
       <c r="AL28" s="47"/>
       <c r="AM28" s="47"/>
-      <c r="AN28" s="48" t="s">
-        <v>40</v>
-      </c>
+      <c r="AN28" s="48"/>
       <c r="AO28" s="48"/>
       <c r="AP28" s="48"/>
       <c r="AQ28" s="48"/>
@@ -28577,9 +28551,7 @@
       <c r="B29" s="45"/>
       <c r="C29" s="46"/>
       <c r="D29" s="41"/>
-      <c r="E29" s="41" t="s">
-        <v>37</v>
-      </c>
+      <c r="E29" s="41"/>
       <c r="F29" s="41"/>
       <c r="G29" s="41"/>
       <c r="H29" s="41"/>
@@ -28602,25 +28574,19 @@
       <c r="Y29" s="41"/>
       <c r="Z29" s="41"/>
       <c r="AA29" s="41"/>
-      <c r="AB29" s="49" t="s">
-        <v>38</v>
-      </c>
+      <c r="AB29" s="49"/>
       <c r="AC29" s="49"/>
       <c r="AD29" s="49"/>
       <c r="AE29" s="49"/>
       <c r="AF29" s="49"/>
       <c r="AG29" s="49"/>
-      <c r="AH29" s="49" t="s">
-        <v>39</v>
-      </c>
+      <c r="AH29" s="49"/>
       <c r="AI29" s="49"/>
       <c r="AJ29" s="49"/>
       <c r="AK29" s="49"/>
       <c r="AL29" s="49"/>
       <c r="AM29" s="49"/>
-      <c r="AN29" s="44" t="s">
-        <v>40</v>
-      </c>
+      <c r="AN29" s="44"/>
       <c r="AO29" s="44"/>
       <c r="AP29" s="44"/>
       <c r="AQ29" s="44"/>
@@ -29611,9 +29577,7 @@
       <c r="B30" s="45"/>
       <c r="C30" s="46"/>
       <c r="D30" s="41"/>
-      <c r="E30" s="41" t="s">
-        <v>37</v>
-      </c>
+      <c r="E30" s="41"/>
       <c r="F30" s="41"/>
       <c r="G30" s="41"/>
       <c r="H30" s="41"/>
@@ -29636,25 +29600,19 @@
       <c r="Y30" s="41"/>
       <c r="Z30" s="41"/>
       <c r="AA30" s="41"/>
-      <c r="AB30" s="49" t="s">
-        <v>38</v>
-      </c>
+      <c r="AB30" s="49"/>
       <c r="AC30" s="49"/>
       <c r="AD30" s="49"/>
       <c r="AE30" s="49"/>
       <c r="AF30" s="49"/>
       <c r="AG30" s="49"/>
-      <c r="AH30" s="51" t="s">
-        <v>39</v>
-      </c>
+      <c r="AH30" s="51"/>
       <c r="AI30" s="51"/>
       <c r="AJ30" s="51"/>
       <c r="AK30" s="51"/>
       <c r="AL30" s="51"/>
       <c r="AM30" s="51"/>
-      <c r="AN30" s="44" t="s">
-        <v>40</v>
-      </c>
+      <c r="AN30" s="44"/>
       <c r="AO30" s="44"/>
       <c r="AP30" s="44"/>
       <c r="AQ30" s="44"/>
@@ -30645,9 +30603,7 @@
       <c r="B31" s="45"/>
       <c r="C31" s="46"/>
       <c r="D31" s="41"/>
-      <c r="E31" s="41" t="s">
-        <v>37</v>
-      </c>
+      <c r="E31" s="41"/>
       <c r="F31" s="41"/>
       <c r="G31" s="41"/>
       <c r="H31" s="41"/>
@@ -30670,25 +30626,19 @@
       <c r="Y31" s="41"/>
       <c r="Z31" s="41"/>
       <c r="AA31" s="41"/>
-      <c r="AB31" s="47" t="s">
-        <v>38</v>
-      </c>
+      <c r="AB31" s="47"/>
       <c r="AC31" s="47"/>
       <c r="AD31" s="47"/>
       <c r="AE31" s="47"/>
       <c r="AF31" s="47"/>
       <c r="AG31" s="47"/>
-      <c r="AH31" s="47" t="s">
-        <v>39</v>
-      </c>
+      <c r="AH31" s="47"/>
       <c r="AI31" s="47"/>
       <c r="AJ31" s="47"/>
       <c r="AK31" s="47"/>
       <c r="AL31" s="47"/>
       <c r="AM31" s="47"/>
-      <c r="AN31" s="48" t="s">
-        <v>40</v>
-      </c>
+      <c r="AN31" s="48"/>
       <c r="AO31" s="48"/>
       <c r="AP31" s="48"/>
       <c r="AQ31" s="48"/>
@@ -31679,9 +31629,7 @@
       <c r="B32" s="45"/>
       <c r="C32" s="46"/>
       <c r="D32" s="41"/>
-      <c r="E32" s="41" t="s">
-        <v>37</v>
-      </c>
+      <c r="E32" s="41"/>
       <c r="F32" s="41"/>
       <c r="G32" s="41"/>
       <c r="H32" s="41"/>
@@ -31704,25 +31652,19 @@
       <c r="Y32" s="41"/>
       <c r="Z32" s="41"/>
       <c r="AA32" s="41"/>
-      <c r="AB32" s="47" t="s">
-        <v>38</v>
-      </c>
+      <c r="AB32" s="47"/>
       <c r="AC32" s="47"/>
       <c r="AD32" s="47"/>
       <c r="AE32" s="47"/>
       <c r="AF32" s="47"/>
       <c r="AG32" s="47"/>
-      <c r="AH32" s="47" t="s">
-        <v>39</v>
-      </c>
+      <c r="AH32" s="47"/>
       <c r="AI32" s="47"/>
       <c r="AJ32" s="47"/>
       <c r="AK32" s="47"/>
       <c r="AL32" s="47"/>
       <c r="AM32" s="47"/>
-      <c r="AN32" s="48" t="s">
-        <v>40</v>
-      </c>
+      <c r="AN32" s="48"/>
       <c r="AO32" s="48"/>
       <c r="AP32" s="48"/>
       <c r="AQ32" s="48"/>
@@ -32713,9 +32655,7 @@
       <c r="B33" s="45"/>
       <c r="C33" s="41"/>
       <c r="D33" s="41"/>
-      <c r="E33" s="41" t="s">
-        <v>37</v>
-      </c>
+      <c r="E33" s="41"/>
       <c r="F33" s="41"/>
       <c r="G33" s="41"/>
       <c r="H33" s="41"/>
@@ -32738,25 +32678,19 @@
       <c r="Y33" s="41"/>
       <c r="Z33" s="41"/>
       <c r="AA33" s="41"/>
-      <c r="AB33" s="49" t="s">
-        <v>38</v>
-      </c>
+      <c r="AB33" s="49"/>
       <c r="AC33" s="49"/>
       <c r="AD33" s="49"/>
       <c r="AE33" s="49"/>
       <c r="AF33" s="49"/>
       <c r="AG33" s="49"/>
-      <c r="AH33" s="49" t="s">
-        <v>39</v>
-      </c>
+      <c r="AH33" s="49"/>
       <c r="AI33" s="49"/>
       <c r="AJ33" s="49"/>
       <c r="AK33" s="49"/>
       <c r="AL33" s="49"/>
       <c r="AM33" s="49"/>
-      <c r="AN33" s="52" t="s">
-        <v>40</v>
-      </c>
+      <c r="AN33" s="52"/>
       <c r="AO33" s="52"/>
       <c r="AP33" s="52"/>
       <c r="AQ33" s="52"/>

</xml_diff>

<commit_message>
deleted nulls in group and add message error if no exist works in index
</commit_message>
<xml_diff>
--- a/ReportOut.xlsx
+++ b/ReportOut.xlsx
@@ -136,10 +136,10 @@
     <t>Avance</t>
   </si>
   <si>
-    <t>Cambio de caps 3</t>
+    <t>Cambio de  3</t>
   </si>
   <si>
-    <t>Marcado de Caps 2.7</t>
+    <t>Marcado de Caps 7.</t>
   </si>
   <si>
     <t>17-04-2017, 2:26 am</t>
@@ -148,10 +148,10 @@
     <t>16-04-2017, 4:26 pm</t>
   </si>
   <si>
-    <t>60%</t>
+    <t>100%</t>
   </si>
   <si>
-    <t>Marcado de Caps 2.9</t>
+    <t>Cambio de  9</t>
   </si>
   <si>
     <t>PARA DETALLES VER EN ESQUEMAS PROXIMA PAGINA</t>
@@ -25310,7 +25310,7 @@
       <c r="C24" s="46"/>
       <c r="D24" s="41"/>
       <c r="E24" s="41" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F24" s="41"/>
       <c r="G24" s="41"/>
@@ -25395,7 +25395,9 @@
       <c r="B25" s="45"/>
       <c r="C25" s="46"/>
       <c r="D25" s="41"/>
-      <c r="E25" s="41"/>
+      <c r="E25" s="41" t="s">
+        <v>37</v>
+      </c>
       <c r="F25" s="41"/>
       <c r="G25" s="41"/>
       <c r="H25" s="41"/>
@@ -25418,19 +25420,25 @@
       <c r="Y25" s="41"/>
       <c r="Z25" s="41"/>
       <c r="AA25" s="41"/>
-      <c r="AB25" s="49"/>
+      <c r="AB25" s="49" t="s">
+        <v>38</v>
+      </c>
       <c r="AC25" s="49"/>
       <c r="AD25" s="49"/>
       <c r="AE25" s="49"/>
       <c r="AF25" s="49"/>
       <c r="AG25" s="49"/>
-      <c r="AH25" s="49"/>
+      <c r="AH25" s="49" t="s">
+        <v>39</v>
+      </c>
       <c r="AI25" s="49"/>
       <c r="AJ25" s="49"/>
       <c r="AK25" s="49"/>
       <c r="AL25" s="49"/>
       <c r="AM25" s="49"/>
-      <c r="AN25" s="44"/>
+      <c r="AN25" s="44" t="s">
+        <v>40</v>
+      </c>
       <c r="AO25" s="44"/>
       <c r="AP25" s="44"/>
       <c r="AQ25" s="44"/>
@@ -25473,7 +25481,9 @@
       <c r="B26" s="45"/>
       <c r="C26" s="46"/>
       <c r="D26" s="41"/>
-      <c r="E26" s="41"/>
+      <c r="E26" s="41" t="s">
+        <v>37</v>
+      </c>
       <c r="F26" s="41"/>
       <c r="G26" s="41"/>
       <c r="H26" s="41"/>
@@ -25496,19 +25506,25 @@
       <c r="Y26" s="41"/>
       <c r="Z26" s="41"/>
       <c r="AA26" s="41"/>
-      <c r="AB26" s="47"/>
+      <c r="AB26" s="47" t="s">
+        <v>38</v>
+      </c>
       <c r="AC26" s="47"/>
       <c r="AD26" s="47"/>
       <c r="AE26" s="47"/>
       <c r="AF26" s="47"/>
       <c r="AG26" s="47"/>
-      <c r="AH26" s="47"/>
+      <c r="AH26" s="47" t="s">
+        <v>39</v>
+      </c>
       <c r="AI26" s="47"/>
       <c r="AJ26" s="47"/>
       <c r="AK26" s="47"/>
       <c r="AL26" s="47"/>
       <c r="AM26" s="47"/>
-      <c r="AN26" s="48"/>
+      <c r="AN26" s="48" t="s">
+        <v>40</v>
+      </c>
       <c r="AO26" s="48"/>
       <c r="AP26" s="48"/>
       <c r="AQ26" s="48"/>
@@ -26498,7 +26514,9 @@
       <c r="A27" s="11"/>
       <c r="B27" s="45"/>
       <c r="C27" s="41"/>
-      <c r="D27" s="41"/>
+      <c r="D27" s="41" t="s">
+        <v>41</v>
+      </c>
       <c r="E27" s="41"/>
       <c r="F27" s="41"/>
       <c r="G27" s="41"/>
@@ -27525,7 +27543,9 @@
       <c r="B28" s="45"/>
       <c r="C28" s="46"/>
       <c r="D28" s="41"/>
-      <c r="E28" s="41"/>
+      <c r="E28" s="41" t="s">
+        <v>37</v>
+      </c>
       <c r="F28" s="41"/>
       <c r="G28" s="41"/>
       <c r="H28" s="41"/>
@@ -27548,19 +27568,25 @@
       <c r="Y28" s="41"/>
       <c r="Z28" s="41"/>
       <c r="AA28" s="41"/>
-      <c r="AB28" s="47"/>
+      <c r="AB28" s="47" t="s">
+        <v>38</v>
+      </c>
       <c r="AC28" s="47"/>
       <c r="AD28" s="47"/>
       <c r="AE28" s="47"/>
       <c r="AF28" s="47"/>
       <c r="AG28" s="47"/>
-      <c r="AH28" s="47"/>
+      <c r="AH28" s="47" t="s">
+        <v>39</v>
+      </c>
       <c r="AI28" s="47"/>
       <c r="AJ28" s="47"/>
       <c r="AK28" s="47"/>
       <c r="AL28" s="47"/>
       <c r="AM28" s="47"/>
-      <c r="AN28" s="48"/>
+      <c r="AN28" s="48" t="s">
+        <v>40</v>
+      </c>
       <c r="AO28" s="48"/>
       <c r="AP28" s="48"/>
       <c r="AQ28" s="48"/>
@@ -28551,7 +28577,9 @@
       <c r="B29" s="45"/>
       <c r="C29" s="46"/>
       <c r="D29" s="41"/>
-      <c r="E29" s="41"/>
+      <c r="E29" s="41" t="s">
+        <v>37</v>
+      </c>
       <c r="F29" s="41"/>
       <c r="G29" s="41"/>
       <c r="H29" s="41"/>
@@ -28574,19 +28602,25 @@
       <c r="Y29" s="41"/>
       <c r="Z29" s="41"/>
       <c r="AA29" s="41"/>
-      <c r="AB29" s="49"/>
+      <c r="AB29" s="49" t="s">
+        <v>38</v>
+      </c>
       <c r="AC29" s="49"/>
       <c r="AD29" s="49"/>
       <c r="AE29" s="49"/>
       <c r="AF29" s="49"/>
       <c r="AG29" s="49"/>
-      <c r="AH29" s="49"/>
+      <c r="AH29" s="49" t="s">
+        <v>39</v>
+      </c>
       <c r="AI29" s="49"/>
       <c r="AJ29" s="49"/>
       <c r="AK29" s="49"/>
       <c r="AL29" s="49"/>
       <c r="AM29" s="49"/>
-      <c r="AN29" s="44"/>
+      <c r="AN29" s="44" t="s">
+        <v>40</v>
+      </c>
       <c r="AO29" s="44"/>
       <c r="AP29" s="44"/>
       <c r="AQ29" s="44"/>
@@ -29577,7 +29611,9 @@
       <c r="B30" s="45"/>
       <c r="C30" s="46"/>
       <c r="D30" s="41"/>
-      <c r="E30" s="41"/>
+      <c r="E30" s="41" t="s">
+        <v>37</v>
+      </c>
       <c r="F30" s="41"/>
       <c r="G30" s="41"/>
       <c r="H30" s="41"/>
@@ -29600,19 +29636,25 @@
       <c r="Y30" s="41"/>
       <c r="Z30" s="41"/>
       <c r="AA30" s="41"/>
-      <c r="AB30" s="49"/>
+      <c r="AB30" s="49" t="s">
+        <v>38</v>
+      </c>
       <c r="AC30" s="49"/>
       <c r="AD30" s="49"/>
       <c r="AE30" s="49"/>
       <c r="AF30" s="49"/>
       <c r="AG30" s="49"/>
-      <c r="AH30" s="51"/>
+      <c r="AH30" s="51" t="s">
+        <v>39</v>
+      </c>
       <c r="AI30" s="51"/>
       <c r="AJ30" s="51"/>
       <c r="AK30" s="51"/>
       <c r="AL30" s="51"/>
       <c r="AM30" s="51"/>
-      <c r="AN30" s="44"/>
+      <c r="AN30" s="44" t="s">
+        <v>40</v>
+      </c>
       <c r="AO30" s="44"/>
       <c r="AP30" s="44"/>
       <c r="AQ30" s="44"/>
@@ -30603,7 +30645,9 @@
       <c r="B31" s="45"/>
       <c r="C31" s="46"/>
       <c r="D31" s="41"/>
-      <c r="E31" s="41"/>
+      <c r="E31" s="41" t="s">
+        <v>37</v>
+      </c>
       <c r="F31" s="41"/>
       <c r="G31" s="41"/>
       <c r="H31" s="41"/>
@@ -30626,19 +30670,25 @@
       <c r="Y31" s="41"/>
       <c r="Z31" s="41"/>
       <c r="AA31" s="41"/>
-      <c r="AB31" s="47"/>
+      <c r="AB31" s="47" t="s">
+        <v>38</v>
+      </c>
       <c r="AC31" s="47"/>
       <c r="AD31" s="47"/>
       <c r="AE31" s="47"/>
       <c r="AF31" s="47"/>
       <c r="AG31" s="47"/>
-      <c r="AH31" s="47"/>
+      <c r="AH31" s="47" t="s">
+        <v>39</v>
+      </c>
       <c r="AI31" s="47"/>
       <c r="AJ31" s="47"/>
       <c r="AK31" s="47"/>
       <c r="AL31" s="47"/>
       <c r="AM31" s="47"/>
-      <c r="AN31" s="48"/>
+      <c r="AN31" s="48" t="s">
+        <v>40</v>
+      </c>
       <c r="AO31" s="48"/>
       <c r="AP31" s="48"/>
       <c r="AQ31" s="48"/>
@@ -31629,7 +31679,9 @@
       <c r="B32" s="45"/>
       <c r="C32" s="46"/>
       <c r="D32" s="41"/>
-      <c r="E32" s="41"/>
+      <c r="E32" s="41" t="s">
+        <v>37</v>
+      </c>
       <c r="F32" s="41"/>
       <c r="G32" s="41"/>
       <c r="H32" s="41"/>
@@ -31652,19 +31704,25 @@
       <c r="Y32" s="41"/>
       <c r="Z32" s="41"/>
       <c r="AA32" s="41"/>
-      <c r="AB32" s="47"/>
+      <c r="AB32" s="47" t="s">
+        <v>38</v>
+      </c>
       <c r="AC32" s="47"/>
       <c r="AD32" s="47"/>
       <c r="AE32" s="47"/>
       <c r="AF32" s="47"/>
       <c r="AG32" s="47"/>
-      <c r="AH32" s="47"/>
+      <c r="AH32" s="47" t="s">
+        <v>39</v>
+      </c>
       <c r="AI32" s="47"/>
       <c r="AJ32" s="47"/>
       <c r="AK32" s="47"/>
       <c r="AL32" s="47"/>
       <c r="AM32" s="47"/>
-      <c r="AN32" s="48"/>
+      <c r="AN32" s="48" t="s">
+        <v>40</v>
+      </c>
       <c r="AO32" s="48"/>
       <c r="AP32" s="48"/>
       <c r="AQ32" s="48"/>

</xml_diff>

<commit_message>
add ver foto in index
</commit_message>
<xml_diff>
--- a/ReportOut.xlsx
+++ b/ReportOut.xlsx
@@ -32713,7 +32713,9 @@
       <c r="B33" s="45"/>
       <c r="C33" s="41"/>
       <c r="D33" s="41"/>
-      <c r="E33" s="41"/>
+      <c r="E33" s="41" t="s">
+        <v>37</v>
+      </c>
       <c r="F33" s="41"/>
       <c r="G33" s="41"/>
       <c r="H33" s="41"/>
@@ -32736,19 +32738,25 @@
       <c r="Y33" s="41"/>
       <c r="Z33" s="41"/>
       <c r="AA33" s="41"/>
-      <c r="AB33" s="49"/>
+      <c r="AB33" s="49" t="s">
+        <v>38</v>
+      </c>
       <c r="AC33" s="49"/>
       <c r="AD33" s="49"/>
       <c r="AE33" s="49"/>
       <c r="AF33" s="49"/>
       <c r="AG33" s="49"/>
-      <c r="AH33" s="49"/>
+      <c r="AH33" s="49" t="s">
+        <v>39</v>
+      </c>
       <c r="AI33" s="49"/>
       <c r="AJ33" s="49"/>
       <c r="AK33" s="49"/>
       <c r="AL33" s="49"/>
       <c r="AM33" s="49"/>
-      <c r="AN33" s="52"/>
+      <c r="AN33" s="52" t="s">
+        <v>40</v>
+      </c>
       <c r="AO33" s="52"/>
       <c r="AP33" s="52"/>
       <c r="AQ33" s="52"/>

</xml_diff>

<commit_message>
fix dsr and der in repor view
</commit_message>
<xml_diff>
--- a/ReportOut.xlsx
+++ b/ReportOut.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="56">
   <si>
     <t>Fabricación, Montaje, Mantención y Reparación</t>
   </si>
@@ -136,7 +136,7 @@
     <t>Avance</t>
   </si>
   <si>
-    <t>Cambio de  3</t>
+    <t>Cambio de  9</t>
   </si>
   <si>
     <t>Marcado de Caps 7.</t>
@@ -149,9 +149,6 @@
   </si>
   <si>
     <t>100%</t>
-  </si>
-  <si>
-    <t>Cambio de  9</t>
   </si>
   <si>
     <t>PARA DETALLES VER EN ESQUEMAS PROXIMA PAGINA</t>
@@ -23241,9 +23238,7 @@
       <c r="B22" s="45"/>
       <c r="C22" s="46"/>
       <c r="D22" s="41"/>
-      <c r="E22" s="41" t="s">
-        <v>37</v>
-      </c>
+      <c r="E22" s="41"/>
       <c r="F22" s="41"/>
       <c r="G22" s="41"/>
       <c r="H22" s="41"/>
@@ -23266,25 +23261,19 @@
       <c r="Y22" s="41"/>
       <c r="Z22" s="41"/>
       <c r="AA22" s="41"/>
-      <c r="AB22" s="49" t="s">
-        <v>38</v>
-      </c>
+      <c r="AB22" s="49"/>
       <c r="AC22" s="49"/>
       <c r="AD22" s="49"/>
       <c r="AE22" s="49"/>
       <c r="AF22" s="49"/>
       <c r="AG22" s="49"/>
-      <c r="AH22" s="49" t="s">
-        <v>39</v>
-      </c>
+      <c r="AH22" s="49"/>
       <c r="AI22" s="49"/>
       <c r="AJ22" s="49"/>
       <c r="AK22" s="49"/>
       <c r="AL22" s="49"/>
       <c r="AM22" s="49"/>
-      <c r="AN22" s="44" t="s">
-        <v>40</v>
-      </c>
+      <c r="AN22" s="44"/>
       <c r="AO22" s="44"/>
       <c r="AP22" s="44"/>
       <c r="AQ22" s="44"/>
@@ -24275,9 +24264,7 @@
       <c r="B23" s="45"/>
       <c r="C23" s="46"/>
       <c r="D23" s="41"/>
-      <c r="E23" s="41" t="s">
-        <v>37</v>
-      </c>
+      <c r="E23" s="41"/>
       <c r="F23" s="41"/>
       <c r="G23" s="41"/>
       <c r="H23" s="41"/>
@@ -24300,25 +24287,19 @@
       <c r="Y23" s="41"/>
       <c r="Z23" s="41"/>
       <c r="AA23" s="41"/>
-      <c r="AB23" s="49" t="s">
-        <v>38</v>
-      </c>
+      <c r="AB23" s="49"/>
       <c r="AC23" s="49"/>
       <c r="AD23" s="49"/>
       <c r="AE23" s="49"/>
       <c r="AF23" s="49"/>
       <c r="AG23" s="49"/>
-      <c r="AH23" s="49" t="s">
-        <v>39</v>
-      </c>
+      <c r="AH23" s="49"/>
       <c r="AI23" s="49"/>
       <c r="AJ23" s="49"/>
       <c r="AK23" s="49"/>
       <c r="AL23" s="49"/>
       <c r="AM23" s="49"/>
-      <c r="AN23" s="44" t="s">
-        <v>40</v>
-      </c>
+      <c r="AN23" s="44"/>
       <c r="AO23" s="44"/>
       <c r="AP23" s="44"/>
       <c r="AQ23" s="44"/>
@@ -25309,9 +25290,7 @@
       <c r="B24" s="45"/>
       <c r="C24" s="46"/>
       <c r="D24" s="41"/>
-      <c r="E24" s="41" t="s">
-        <v>37</v>
-      </c>
+      <c r="E24" s="41"/>
       <c r="F24" s="41"/>
       <c r="G24" s="41"/>
       <c r="H24" s="41"/>
@@ -25334,25 +25313,19 @@
       <c r="Y24" s="41"/>
       <c r="Z24" s="41"/>
       <c r="AA24" s="41"/>
-      <c r="AB24" s="49" t="s">
-        <v>38</v>
-      </c>
+      <c r="AB24" s="49"/>
       <c r="AC24" s="49"/>
       <c r="AD24" s="49"/>
       <c r="AE24" s="49"/>
       <c r="AF24" s="49"/>
       <c r="AG24" s="49"/>
-      <c r="AH24" s="49" t="s">
-        <v>39</v>
-      </c>
+      <c r="AH24" s="49"/>
       <c r="AI24" s="49"/>
       <c r="AJ24" s="49"/>
       <c r="AK24" s="49"/>
       <c r="AL24" s="49"/>
       <c r="AM24" s="49"/>
-      <c r="AN24" s="44" t="s">
-        <v>40</v>
-      </c>
+      <c r="AN24" s="44"/>
       <c r="AO24" s="44"/>
       <c r="AP24" s="44"/>
       <c r="AQ24" s="44"/>
@@ -25395,9 +25368,7 @@
       <c r="B25" s="45"/>
       <c r="C25" s="46"/>
       <c r="D25" s="41"/>
-      <c r="E25" s="41" t="s">
-        <v>37</v>
-      </c>
+      <c r="E25" s="41"/>
       <c r="F25" s="41"/>
       <c r="G25" s="41"/>
       <c r="H25" s="41"/>
@@ -25420,25 +25391,19 @@
       <c r="Y25" s="41"/>
       <c r="Z25" s="41"/>
       <c r="AA25" s="41"/>
-      <c r="AB25" s="49" t="s">
-        <v>38</v>
-      </c>
+      <c r="AB25" s="49"/>
       <c r="AC25" s="49"/>
       <c r="AD25" s="49"/>
       <c r="AE25" s="49"/>
       <c r="AF25" s="49"/>
       <c r="AG25" s="49"/>
-      <c r="AH25" s="49" t="s">
-        <v>39</v>
-      </c>
+      <c r="AH25" s="49"/>
       <c r="AI25" s="49"/>
       <c r="AJ25" s="49"/>
       <c r="AK25" s="49"/>
       <c r="AL25" s="49"/>
       <c r="AM25" s="49"/>
-      <c r="AN25" s="44" t="s">
-        <v>40</v>
-      </c>
+      <c r="AN25" s="44"/>
       <c r="AO25" s="44"/>
       <c r="AP25" s="44"/>
       <c r="AQ25" s="44"/>
@@ -25481,9 +25446,7 @@
       <c r="B26" s="45"/>
       <c r="C26" s="46"/>
       <c r="D26" s="41"/>
-      <c r="E26" s="41" t="s">
-        <v>37</v>
-      </c>
+      <c r="E26" s="41"/>
       <c r="F26" s="41"/>
       <c r="G26" s="41"/>
       <c r="H26" s="41"/>
@@ -25506,25 +25469,19 @@
       <c r="Y26" s="41"/>
       <c r="Z26" s="41"/>
       <c r="AA26" s="41"/>
-      <c r="AB26" s="47" t="s">
-        <v>38</v>
-      </c>
+      <c r="AB26" s="47"/>
       <c r="AC26" s="47"/>
       <c r="AD26" s="47"/>
       <c r="AE26" s="47"/>
       <c r="AF26" s="47"/>
       <c r="AG26" s="47"/>
-      <c r="AH26" s="47" t="s">
-        <v>39</v>
-      </c>
+      <c r="AH26" s="47"/>
       <c r="AI26" s="47"/>
       <c r="AJ26" s="47"/>
       <c r="AK26" s="47"/>
       <c r="AL26" s="47"/>
       <c r="AM26" s="47"/>
-      <c r="AN26" s="48" t="s">
-        <v>40</v>
-      </c>
+      <c r="AN26" s="48"/>
       <c r="AO26" s="48"/>
       <c r="AP26" s="48"/>
       <c r="AQ26" s="48"/>
@@ -26514,9 +26471,7 @@
       <c r="A27" s="11"/>
       <c r="B27" s="45"/>
       <c r="C27" s="41"/>
-      <c r="D27" s="41" t="s">
-        <v>41</v>
-      </c>
+      <c r="D27" s="41"/>
       <c r="E27" s="41"/>
       <c r="F27" s="41"/>
       <c r="G27" s="41"/>
@@ -27543,9 +27498,7 @@
       <c r="B28" s="45"/>
       <c r="C28" s="46"/>
       <c r="D28" s="41"/>
-      <c r="E28" s="41" t="s">
-        <v>37</v>
-      </c>
+      <c r="E28" s="41"/>
       <c r="F28" s="41"/>
       <c r="G28" s="41"/>
       <c r="H28" s="41"/>
@@ -27568,25 +27521,19 @@
       <c r="Y28" s="41"/>
       <c r="Z28" s="41"/>
       <c r="AA28" s="41"/>
-      <c r="AB28" s="47" t="s">
-        <v>38</v>
-      </c>
+      <c r="AB28" s="47"/>
       <c r="AC28" s="47"/>
       <c r="AD28" s="47"/>
       <c r="AE28" s="47"/>
       <c r="AF28" s="47"/>
       <c r="AG28" s="47"/>
-      <c r="AH28" s="47" t="s">
-        <v>39</v>
-      </c>
+      <c r="AH28" s="47"/>
       <c r="AI28" s="47"/>
       <c r="AJ28" s="47"/>
       <c r="AK28" s="47"/>
       <c r="AL28" s="47"/>
       <c r="AM28" s="47"/>
-      <c r="AN28" s="48" t="s">
-        <v>40</v>
-      </c>
+      <c r="AN28" s="48"/>
       <c r="AO28" s="48"/>
       <c r="AP28" s="48"/>
       <c r="AQ28" s="48"/>
@@ -28577,9 +28524,7 @@
       <c r="B29" s="45"/>
       <c r="C29" s="46"/>
       <c r="D29" s="41"/>
-      <c r="E29" s="41" t="s">
-        <v>37</v>
-      </c>
+      <c r="E29" s="41"/>
       <c r="F29" s="41"/>
       <c r="G29" s="41"/>
       <c r="H29" s="41"/>
@@ -28602,25 +28547,19 @@
       <c r="Y29" s="41"/>
       <c r="Z29" s="41"/>
       <c r="AA29" s="41"/>
-      <c r="AB29" s="49" t="s">
-        <v>38</v>
-      </c>
+      <c r="AB29" s="49"/>
       <c r="AC29" s="49"/>
       <c r="AD29" s="49"/>
       <c r="AE29" s="49"/>
       <c r="AF29" s="49"/>
       <c r="AG29" s="49"/>
-      <c r="AH29" s="49" t="s">
-        <v>39</v>
-      </c>
+      <c r="AH29" s="49"/>
       <c r="AI29" s="49"/>
       <c r="AJ29" s="49"/>
       <c r="AK29" s="49"/>
       <c r="AL29" s="49"/>
       <c r="AM29" s="49"/>
-      <c r="AN29" s="44" t="s">
-        <v>40</v>
-      </c>
+      <c r="AN29" s="44"/>
       <c r="AO29" s="44"/>
       <c r="AP29" s="44"/>
       <c r="AQ29" s="44"/>
@@ -29611,9 +29550,7 @@
       <c r="B30" s="45"/>
       <c r="C30" s="46"/>
       <c r="D30" s="41"/>
-      <c r="E30" s="41" t="s">
-        <v>37</v>
-      </c>
+      <c r="E30" s="41"/>
       <c r="F30" s="41"/>
       <c r="G30" s="41"/>
       <c r="H30" s="41"/>
@@ -29636,25 +29573,19 @@
       <c r="Y30" s="41"/>
       <c r="Z30" s="41"/>
       <c r="AA30" s="41"/>
-      <c r="AB30" s="49" t="s">
-        <v>38</v>
-      </c>
+      <c r="AB30" s="49"/>
       <c r="AC30" s="49"/>
       <c r="AD30" s="49"/>
       <c r="AE30" s="49"/>
       <c r="AF30" s="49"/>
       <c r="AG30" s="49"/>
-      <c r="AH30" s="51" t="s">
-        <v>39</v>
-      </c>
+      <c r="AH30" s="51"/>
       <c r="AI30" s="51"/>
       <c r="AJ30" s="51"/>
       <c r="AK30" s="51"/>
       <c r="AL30" s="51"/>
       <c r="AM30" s="51"/>
-      <c r="AN30" s="44" t="s">
-        <v>40</v>
-      </c>
+      <c r="AN30" s="44"/>
       <c r="AO30" s="44"/>
       <c r="AP30" s="44"/>
       <c r="AQ30" s="44"/>
@@ -30645,9 +30576,7 @@
       <c r="B31" s="45"/>
       <c r="C31" s="46"/>
       <c r="D31" s="41"/>
-      <c r="E31" s="41" t="s">
-        <v>37</v>
-      </c>
+      <c r="E31" s="41"/>
       <c r="F31" s="41"/>
       <c r="G31" s="41"/>
       <c r="H31" s="41"/>
@@ -30670,25 +30599,19 @@
       <c r="Y31" s="41"/>
       <c r="Z31" s="41"/>
       <c r="AA31" s="41"/>
-      <c r="AB31" s="47" t="s">
-        <v>38</v>
-      </c>
+      <c r="AB31" s="47"/>
       <c r="AC31" s="47"/>
       <c r="AD31" s="47"/>
       <c r="AE31" s="47"/>
       <c r="AF31" s="47"/>
       <c r="AG31" s="47"/>
-      <c r="AH31" s="47" t="s">
-        <v>39</v>
-      </c>
+      <c r="AH31" s="47"/>
       <c r="AI31" s="47"/>
       <c r="AJ31" s="47"/>
       <c r="AK31" s="47"/>
       <c r="AL31" s="47"/>
       <c r="AM31" s="47"/>
-      <c r="AN31" s="48" t="s">
-        <v>40</v>
-      </c>
+      <c r="AN31" s="48"/>
       <c r="AO31" s="48"/>
       <c r="AP31" s="48"/>
       <c r="AQ31" s="48"/>
@@ -31679,9 +31602,7 @@
       <c r="B32" s="45"/>
       <c r="C32" s="46"/>
       <c r="D32" s="41"/>
-      <c r="E32" s="41" t="s">
-        <v>37</v>
-      </c>
+      <c r="E32" s="41"/>
       <c r="F32" s="41"/>
       <c r="G32" s="41"/>
       <c r="H32" s="41"/>
@@ -31704,25 +31625,19 @@
       <c r="Y32" s="41"/>
       <c r="Z32" s="41"/>
       <c r="AA32" s="41"/>
-      <c r="AB32" s="47" t="s">
-        <v>38</v>
-      </c>
+      <c r="AB32" s="47"/>
       <c r="AC32" s="47"/>
       <c r="AD32" s="47"/>
       <c r="AE32" s="47"/>
       <c r="AF32" s="47"/>
       <c r="AG32" s="47"/>
-      <c r="AH32" s="47" t="s">
-        <v>39</v>
-      </c>
+      <c r="AH32" s="47"/>
       <c r="AI32" s="47"/>
       <c r="AJ32" s="47"/>
       <c r="AK32" s="47"/>
       <c r="AL32" s="47"/>
       <c r="AM32" s="47"/>
-      <c r="AN32" s="48" t="s">
-        <v>40</v>
-      </c>
+      <c r="AN32" s="48"/>
       <c r="AO32" s="48"/>
       <c r="AP32" s="48"/>
       <c r="AQ32" s="48"/>
@@ -32713,9 +32628,7 @@
       <c r="B33" s="45"/>
       <c r="C33" s="41"/>
       <c r="D33" s="41"/>
-      <c r="E33" s="41" t="s">
-        <v>37</v>
-      </c>
+      <c r="E33" s="41"/>
       <c r="F33" s="41"/>
       <c r="G33" s="41"/>
       <c r="H33" s="41"/>
@@ -32738,25 +32651,19 @@
       <c r="Y33" s="41"/>
       <c r="Z33" s="41"/>
       <c r="AA33" s="41"/>
-      <c r="AB33" s="49" t="s">
-        <v>38</v>
-      </c>
+      <c r="AB33" s="49"/>
       <c r="AC33" s="49"/>
       <c r="AD33" s="49"/>
       <c r="AE33" s="49"/>
       <c r="AF33" s="49"/>
       <c r="AG33" s="49"/>
-      <c r="AH33" s="49" t="s">
-        <v>39</v>
-      </c>
+      <c r="AH33" s="49"/>
       <c r="AI33" s="49"/>
       <c r="AJ33" s="49"/>
       <c r="AK33" s="49"/>
       <c r="AL33" s="49"/>
       <c r="AM33" s="49"/>
-      <c r="AN33" s="52" t="s">
-        <v>40</v>
-      </c>
+      <c r="AN33" s="52"/>
       <c r="AO33" s="52"/>
       <c r="AP33" s="52"/>
       <c r="AQ33" s="52"/>
@@ -42979,7 +42886,7 @@
     <row r="43" spans="1:1025" customHeight="1" ht="15">
       <c r="A43" s="11"/>
       <c r="B43" s="58" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C43" s="58"/>
       <c r="D43" s="58"/>
@@ -44007,7 +43914,7 @@
     <row r="44" spans="1:1025" customHeight="1" ht="15">
       <c r="A44" s="11"/>
       <c r="B44" s="26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C44" s="26"/>
       <c r="D44" s="26"/>
@@ -44044,7 +43951,7 @@
       <c r="AI44" s="26"/>
       <c r="AJ44" s="26"/>
       <c r="AK44" s="27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AL44" s="27"/>
       <c r="AM44" s="27"/>
@@ -45038,7 +44945,7 @@
       <c r="A45" s="11"/>
       <c r="B45" s="59"/>
       <c r="C45" s="60" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D45" s="60"/>
       <c r="E45" s="61"/>
@@ -46066,7 +45973,7 @@
       <c r="A46" s="11"/>
       <c r="B46" s="59"/>
       <c r="C46" s="61" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D46" s="61"/>
       <c r="E46" s="61"/>
@@ -47094,7 +47001,7 @@
       <c r="A47" s="11"/>
       <c r="B47" s="65"/>
       <c r="C47" s="66" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D47" s="66"/>
       <c r="E47" s="66"/>
@@ -48121,7 +48028,7 @@
     <row r="48" spans="1:1025" customHeight="1" ht="15">
       <c r="A48" s="11"/>
       <c r="B48" s="69" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C48" s="69"/>
       <c r="D48" s="69"/>
@@ -49149,11 +49056,11 @@
     <row r="49" spans="1:1025" customHeight="1" ht="15">
       <c r="A49" s="11"/>
       <c r="B49" s="70" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C49" s="70"/>
       <c r="D49" s="71" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E49" s="71"/>
       <c r="F49" s="71"/>
@@ -49167,11 +49074,11 @@
       <c r="N49" s="71"/>
       <c r="O49" s="71"/>
       <c r="P49" s="72" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q49" s="72"/>
       <c r="R49" s="71" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="S49" s="71"/>
       <c r="T49" s="71"/>
@@ -49185,11 +49092,11 @@
       <c r="AB49" s="71"/>
       <c r="AC49" s="71"/>
       <c r="AD49" s="72" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AE49" s="72"/>
       <c r="AF49" s="71" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AG49" s="71"/>
       <c r="AH49" s="71"/>
@@ -63569,11 +63476,11 @@
     <row r="64" spans="1:1025" customHeight="1" ht="15">
       <c r="A64"/>
       <c r="B64" s="70" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C64" s="70"/>
       <c r="D64" s="71" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E64" s="71"/>
       <c r="F64" s="71"/>
@@ -63587,11 +63494,11 @@
       <c r="N64" s="71"/>
       <c r="O64" s="71"/>
       <c r="P64" s="72" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q64" s="72"/>
       <c r="R64" s="71" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="S64" s="71"/>
       <c r="T64" s="71"/>
@@ -63605,11 +63512,11 @@
       <c r="AB64" s="71"/>
       <c r="AC64" s="71"/>
       <c r="AD64" s="72" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AE64" s="72"/>
       <c r="AF64" s="78" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AG64" s="78"/>
       <c r="AH64" s="78"/>

</xml_diff>

<commit_message>
fix prueba dsr der
</commit_message>
<xml_diff>
--- a/ReportOut.xlsx
+++ b/ReportOut.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="58">
   <si>
     <t>Fabricación, Montaje, Mantención y Reparación</t>
   </si>
@@ -149,6 +149,12 @@
   </si>
   <si>
     <t>100%</t>
+  </si>
+  <si>
+    <t>16-04-2017, 11:26 pm</t>
+  </si>
+  <si>
+    <t>16-04-2017, 1:26 pm</t>
   </si>
   <si>
     <t>PARA DETALLES VER EN ESQUEMAS PROXIMA PAGINA</t>
@@ -23238,7 +23244,9 @@
       <c r="B22" s="45"/>
       <c r="C22" s="46"/>
       <c r="D22" s="41"/>
-      <c r="E22" s="41"/>
+      <c r="E22" s="41" t="s">
+        <v>37</v>
+      </c>
       <c r="F22" s="41"/>
       <c r="G22" s="41"/>
       <c r="H22" s="41"/>
@@ -23261,19 +23269,25 @@
       <c r="Y22" s="41"/>
       <c r="Z22" s="41"/>
       <c r="AA22" s="41"/>
-      <c r="AB22" s="49"/>
+      <c r="AB22" s="49" t="s">
+        <v>41</v>
+      </c>
       <c r="AC22" s="49"/>
       <c r="AD22" s="49"/>
       <c r="AE22" s="49"/>
       <c r="AF22" s="49"/>
       <c r="AG22" s="49"/>
-      <c r="AH22" s="49"/>
+      <c r="AH22" s="49" t="s">
+        <v>42</v>
+      </c>
       <c r="AI22" s="49"/>
       <c r="AJ22" s="49"/>
       <c r="AK22" s="49"/>
       <c r="AL22" s="49"/>
       <c r="AM22" s="49"/>
-      <c r="AN22" s="44"/>
+      <c r="AN22" s="44" t="s">
+        <v>40</v>
+      </c>
       <c r="AO22" s="44"/>
       <c r="AP22" s="44"/>
       <c r="AQ22" s="44"/>
@@ -42886,7 +42900,7 @@
     <row r="43" spans="1:1025" customHeight="1" ht="15">
       <c r="A43" s="11"/>
       <c r="B43" s="58" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C43" s="58"/>
       <c r="D43" s="58"/>
@@ -43914,7 +43928,7 @@
     <row r="44" spans="1:1025" customHeight="1" ht="15">
       <c r="A44" s="11"/>
       <c r="B44" s="26" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C44" s="26"/>
       <c r="D44" s="26"/>
@@ -43951,7 +43965,7 @@
       <c r="AI44" s="26"/>
       <c r="AJ44" s="26"/>
       <c r="AK44" s="27" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="AL44" s="27"/>
       <c r="AM44" s="27"/>
@@ -44945,7 +44959,7 @@
       <c r="A45" s="11"/>
       <c r="B45" s="59"/>
       <c r="C45" s="60" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D45" s="60"/>
       <c r="E45" s="61"/>
@@ -45973,7 +45987,7 @@
       <c r="A46" s="11"/>
       <c r="B46" s="59"/>
       <c r="C46" s="61" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D46" s="61"/>
       <c r="E46" s="61"/>
@@ -47001,7 +47015,7 @@
       <c r="A47" s="11"/>
       <c r="B47" s="65"/>
       <c r="C47" s="66" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D47" s="66"/>
       <c r="E47" s="66"/>
@@ -48028,7 +48042,7 @@
     <row r="48" spans="1:1025" customHeight="1" ht="15">
       <c r="A48" s="11"/>
       <c r="B48" s="69" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C48" s="69"/>
       <c r="D48" s="69"/>
@@ -49056,11 +49070,11 @@
     <row r="49" spans="1:1025" customHeight="1" ht="15">
       <c r="A49" s="11"/>
       <c r="B49" s="70" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C49" s="70"/>
       <c r="D49" s="71" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E49" s="71"/>
       <c r="F49" s="71"/>
@@ -49074,11 +49088,11 @@
       <c r="N49" s="71"/>
       <c r="O49" s="71"/>
       <c r="P49" s="72" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="Q49" s="72"/>
       <c r="R49" s="71" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="S49" s="71"/>
       <c r="T49" s="71"/>
@@ -49092,11 +49106,11 @@
       <c r="AB49" s="71"/>
       <c r="AC49" s="71"/>
       <c r="AD49" s="72" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AE49" s="72"/>
       <c r="AF49" s="71" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AG49" s="71"/>
       <c r="AH49" s="71"/>
@@ -63476,11 +63490,11 @@
     <row r="64" spans="1:1025" customHeight="1" ht="15">
       <c r="A64"/>
       <c r="B64" s="70" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C64" s="70"/>
       <c r="D64" s="71" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E64" s="71"/>
       <c r="F64" s="71"/>
@@ -63494,11 +63508,11 @@
       <c r="N64" s="71"/>
       <c r="O64" s="71"/>
       <c r="P64" s="72" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="Q64" s="72"/>
       <c r="R64" s="71" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="S64" s="71"/>
       <c r="T64" s="71"/>
@@ -63512,11 +63526,11 @@
       <c r="AB64" s="71"/>
       <c r="AC64" s="71"/>
       <c r="AD64" s="72" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AE64" s="72"/>
       <c r="AF64" s="78" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="AG64" s="78"/>
       <c r="AH64" s="78"/>

</xml_diff>

<commit_message>
fix des and der to america/santiago
</commit_message>
<xml_diff>
--- a/ReportOut.xlsx
+++ b/ReportOut.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="59">
   <si>
     <t>Fabricación, Montaje, Mantención y Reparación</t>
   </si>
@@ -142,7 +142,7 @@
     <t>Marcado de Caps 7.</t>
   </si>
   <si>
-    <t>17-04-2017, 2:26 am</t>
+    <t>18-04-2017, 2:26 am</t>
   </si>
   <si>
     <t>16-04-2017, 4:26 pm</t>
@@ -151,7 +151,10 @@
     <t>100%</t>
   </si>
   <si>
-    <t>16-04-2017, 11:26 pm</t>
+    <t>Cambio de  1</t>
+  </si>
+  <si>
+    <t>17-04-2017, 11:26 pm</t>
   </si>
   <si>
     <t>16-04-2017, 1:26 pm</t>
@@ -23243,10 +23246,10 @@
       <c r="A22" s="12"/>
       <c r="B22" s="45"/>
       <c r="C22" s="46"/>
-      <c r="D22" s="41"/>
-      <c r="E22" s="41" t="s">
-        <v>37</v>
+      <c r="D22" s="41" t="s">
+        <v>41</v>
       </c>
+      <c r="E22" s="41"/>
       <c r="F22" s="41"/>
       <c r="G22" s="41"/>
       <c r="H22" s="41"/>
@@ -23269,25 +23272,19 @@
       <c r="Y22" s="41"/>
       <c r="Z22" s="41"/>
       <c r="AA22" s="41"/>
-      <c r="AB22" s="49" t="s">
-        <v>41</v>
-      </c>
+      <c r="AB22" s="49"/>
       <c r="AC22" s="49"/>
       <c r="AD22" s="49"/>
       <c r="AE22" s="49"/>
       <c r="AF22" s="49"/>
       <c r="AG22" s="49"/>
-      <c r="AH22" s="49" t="s">
-        <v>42</v>
-      </c>
+      <c r="AH22" s="49"/>
       <c r="AI22" s="49"/>
       <c r="AJ22" s="49"/>
       <c r="AK22" s="49"/>
       <c r="AL22" s="49"/>
       <c r="AM22" s="49"/>
-      <c r="AN22" s="44" t="s">
-        <v>40</v>
-      </c>
+      <c r="AN22" s="44"/>
       <c r="AO22" s="44"/>
       <c r="AP22" s="44"/>
       <c r="AQ22" s="44"/>
@@ -24278,7 +24275,9 @@
       <c r="B23" s="45"/>
       <c r="C23" s="46"/>
       <c r="D23" s="41"/>
-      <c r="E23" s="41"/>
+      <c r="E23" s="41" t="s">
+        <v>37</v>
+      </c>
       <c r="F23" s="41"/>
       <c r="G23" s="41"/>
       <c r="H23" s="41"/>
@@ -24301,19 +24300,25 @@
       <c r="Y23" s="41"/>
       <c r="Z23" s="41"/>
       <c r="AA23" s="41"/>
-      <c r="AB23" s="49"/>
+      <c r="AB23" s="49" t="s">
+        <v>42</v>
+      </c>
       <c r="AC23" s="49"/>
       <c r="AD23" s="49"/>
       <c r="AE23" s="49"/>
       <c r="AF23" s="49"/>
       <c r="AG23" s="49"/>
-      <c r="AH23" s="49"/>
+      <c r="AH23" s="49" t="s">
+        <v>43</v>
+      </c>
       <c r="AI23" s="49"/>
       <c r="AJ23" s="49"/>
       <c r="AK23" s="49"/>
       <c r="AL23" s="49"/>
       <c r="AM23" s="49"/>
-      <c r="AN23" s="44"/>
+      <c r="AN23" s="44" t="s">
+        <v>40</v>
+      </c>
       <c r="AO23" s="44"/>
       <c r="AP23" s="44"/>
       <c r="AQ23" s="44"/>
@@ -25304,7 +25309,9 @@
       <c r="B24" s="45"/>
       <c r="C24" s="46"/>
       <c r="D24" s="41"/>
-      <c r="E24" s="41"/>
+      <c r="E24" s="41" t="s">
+        <v>37</v>
+      </c>
       <c r="F24" s="41"/>
       <c r="G24" s="41"/>
       <c r="H24" s="41"/>
@@ -25327,19 +25334,25 @@
       <c r="Y24" s="41"/>
       <c r="Z24" s="41"/>
       <c r="AA24" s="41"/>
-      <c r="AB24" s="49"/>
+      <c r="AB24" s="49" t="s">
+        <v>42</v>
+      </c>
       <c r="AC24" s="49"/>
       <c r="AD24" s="49"/>
       <c r="AE24" s="49"/>
       <c r="AF24" s="49"/>
       <c r="AG24" s="49"/>
-      <c r="AH24" s="49"/>
+      <c r="AH24" s="49" t="s">
+        <v>43</v>
+      </c>
       <c r="AI24" s="49"/>
       <c r="AJ24" s="49"/>
       <c r="AK24" s="49"/>
       <c r="AL24" s="49"/>
       <c r="AM24" s="49"/>
-      <c r="AN24" s="44"/>
+      <c r="AN24" s="44" t="s">
+        <v>40</v>
+      </c>
       <c r="AO24" s="44"/>
       <c r="AP24" s="44"/>
       <c r="AQ24" s="44"/>
@@ -25382,7 +25395,9 @@
       <c r="B25" s="45"/>
       <c r="C25" s="46"/>
       <c r="D25" s="41"/>
-      <c r="E25" s="41"/>
+      <c r="E25" s="41" t="s">
+        <v>37</v>
+      </c>
       <c r="F25" s="41"/>
       <c r="G25" s="41"/>
       <c r="H25" s="41"/>
@@ -25405,19 +25420,25 @@
       <c r="Y25" s="41"/>
       <c r="Z25" s="41"/>
       <c r="AA25" s="41"/>
-      <c r="AB25" s="49"/>
+      <c r="AB25" s="49" t="s">
+        <v>42</v>
+      </c>
       <c r="AC25" s="49"/>
       <c r="AD25" s="49"/>
       <c r="AE25" s="49"/>
       <c r="AF25" s="49"/>
       <c r="AG25" s="49"/>
-      <c r="AH25" s="49"/>
+      <c r="AH25" s="49" t="s">
+        <v>43</v>
+      </c>
       <c r="AI25" s="49"/>
       <c r="AJ25" s="49"/>
       <c r="AK25" s="49"/>
       <c r="AL25" s="49"/>
       <c r="AM25" s="49"/>
-      <c r="AN25" s="44"/>
+      <c r="AN25" s="44" t="s">
+        <v>40</v>
+      </c>
       <c r="AO25" s="44"/>
       <c r="AP25" s="44"/>
       <c r="AQ25" s="44"/>
@@ -25460,7 +25481,9 @@
       <c r="B26" s="45"/>
       <c r="C26" s="46"/>
       <c r="D26" s="41"/>
-      <c r="E26" s="41"/>
+      <c r="E26" s="41" t="s">
+        <v>37</v>
+      </c>
       <c r="F26" s="41"/>
       <c r="G26" s="41"/>
       <c r="H26" s="41"/>
@@ -25483,19 +25506,25 @@
       <c r="Y26" s="41"/>
       <c r="Z26" s="41"/>
       <c r="AA26" s="41"/>
-      <c r="AB26" s="47"/>
+      <c r="AB26" s="47" t="s">
+        <v>42</v>
+      </c>
       <c r="AC26" s="47"/>
       <c r="AD26" s="47"/>
       <c r="AE26" s="47"/>
       <c r="AF26" s="47"/>
       <c r="AG26" s="47"/>
-      <c r="AH26" s="47"/>
+      <c r="AH26" s="47" t="s">
+        <v>43</v>
+      </c>
       <c r="AI26" s="47"/>
       <c r="AJ26" s="47"/>
       <c r="AK26" s="47"/>
       <c r="AL26" s="47"/>
       <c r="AM26" s="47"/>
-      <c r="AN26" s="48"/>
+      <c r="AN26" s="48" t="s">
+        <v>40</v>
+      </c>
       <c r="AO26" s="48"/>
       <c r="AP26" s="48"/>
       <c r="AQ26" s="48"/>
@@ -26486,7 +26515,9 @@
       <c r="B27" s="45"/>
       <c r="C27" s="41"/>
       <c r="D27" s="41"/>
-      <c r="E27" s="41"/>
+      <c r="E27" s="41" t="s">
+        <v>37</v>
+      </c>
       <c r="F27" s="41"/>
       <c r="G27" s="41"/>
       <c r="H27" s="41"/>
@@ -26509,19 +26540,25 @@
       <c r="Y27" s="41"/>
       <c r="Z27" s="41"/>
       <c r="AA27" s="41"/>
-      <c r="AB27" s="49"/>
+      <c r="AB27" s="49" t="s">
+        <v>42</v>
+      </c>
       <c r="AC27" s="49"/>
       <c r="AD27" s="49"/>
       <c r="AE27" s="49"/>
       <c r="AF27" s="49"/>
       <c r="AG27" s="49"/>
-      <c r="AH27" s="49"/>
+      <c r="AH27" s="49" t="s">
+        <v>43</v>
+      </c>
       <c r="AI27" s="49"/>
       <c r="AJ27" s="49"/>
       <c r="AK27" s="49"/>
       <c r="AL27" s="49"/>
       <c r="AM27" s="49"/>
-      <c r="AN27" s="44"/>
+      <c r="AN27" s="44" t="s">
+        <v>40</v>
+      </c>
       <c r="AO27" s="44"/>
       <c r="AP27" s="44"/>
       <c r="AQ27" s="44"/>
@@ -27512,7 +27549,9 @@
       <c r="B28" s="45"/>
       <c r="C28" s="46"/>
       <c r="D28" s="41"/>
-      <c r="E28" s="41"/>
+      <c r="E28" s="41" t="s">
+        <v>37</v>
+      </c>
       <c r="F28" s="41"/>
       <c r="G28" s="41"/>
       <c r="H28" s="41"/>
@@ -27535,19 +27574,25 @@
       <c r="Y28" s="41"/>
       <c r="Z28" s="41"/>
       <c r="AA28" s="41"/>
-      <c r="AB28" s="47"/>
+      <c r="AB28" s="47" t="s">
+        <v>42</v>
+      </c>
       <c r="AC28" s="47"/>
       <c r="AD28" s="47"/>
       <c r="AE28" s="47"/>
       <c r="AF28" s="47"/>
       <c r="AG28" s="47"/>
-      <c r="AH28" s="47"/>
+      <c r="AH28" s="47" t="s">
+        <v>43</v>
+      </c>
       <c r="AI28" s="47"/>
       <c r="AJ28" s="47"/>
       <c r="AK28" s="47"/>
       <c r="AL28" s="47"/>
       <c r="AM28" s="47"/>
-      <c r="AN28" s="48"/>
+      <c r="AN28" s="48" t="s">
+        <v>40</v>
+      </c>
       <c r="AO28" s="48"/>
       <c r="AP28" s="48"/>
       <c r="AQ28" s="48"/>
@@ -42900,7 +42945,7 @@
     <row r="43" spans="1:1025" customHeight="1" ht="15">
       <c r="A43" s="11"/>
       <c r="B43" s="58" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C43" s="58"/>
       <c r="D43" s="58"/>
@@ -43928,7 +43973,7 @@
     <row r="44" spans="1:1025" customHeight="1" ht="15">
       <c r="A44" s="11"/>
       <c r="B44" s="26" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C44" s="26"/>
       <c r="D44" s="26"/>
@@ -43965,7 +44010,7 @@
       <c r="AI44" s="26"/>
       <c r="AJ44" s="26"/>
       <c r="AK44" s="27" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AL44" s="27"/>
       <c r="AM44" s="27"/>
@@ -44959,7 +45004,7 @@
       <c r="A45" s="11"/>
       <c r="B45" s="59"/>
       <c r="C45" s="60" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D45" s="60"/>
       <c r="E45" s="61"/>
@@ -45987,7 +46032,7 @@
       <c r="A46" s="11"/>
       <c r="B46" s="59"/>
       <c r="C46" s="61" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D46" s="61"/>
       <c r="E46" s="61"/>
@@ -47015,7 +47060,7 @@
       <c r="A47" s="11"/>
       <c r="B47" s="65"/>
       <c r="C47" s="66" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D47" s="66"/>
       <c r="E47" s="66"/>
@@ -48042,7 +48087,7 @@
     <row r="48" spans="1:1025" customHeight="1" ht="15">
       <c r="A48" s="11"/>
       <c r="B48" s="69" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C48" s="69"/>
       <c r="D48" s="69"/>
@@ -49070,11 +49115,11 @@
     <row r="49" spans="1:1025" customHeight="1" ht="15">
       <c r="A49" s="11"/>
       <c r="B49" s="70" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C49" s="70"/>
       <c r="D49" s="71" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E49" s="71"/>
       <c r="F49" s="71"/>
@@ -49088,11 +49133,11 @@
       <c r="N49" s="71"/>
       <c r="O49" s="71"/>
       <c r="P49" s="72" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="Q49" s="72"/>
       <c r="R49" s="71" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="S49" s="71"/>
       <c r="T49" s="71"/>
@@ -49106,11 +49151,11 @@
       <c r="AB49" s="71"/>
       <c r="AC49" s="71"/>
       <c r="AD49" s="72" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AE49" s="72"/>
       <c r="AF49" s="71" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AG49" s="71"/>
       <c r="AH49" s="71"/>
@@ -63490,11 +63535,11 @@
     <row r="64" spans="1:1025" customHeight="1" ht="15">
       <c r="A64"/>
       <c r="B64" s="70" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C64" s="70"/>
       <c r="D64" s="71" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E64" s="71"/>
       <c r="F64" s="71"/>
@@ -63508,11 +63553,11 @@
       <c r="N64" s="71"/>
       <c r="O64" s="71"/>
       <c r="P64" s="72" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="Q64" s="72"/>
       <c r="R64" s="71" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="S64" s="71"/>
       <c r="T64" s="71"/>
@@ -63526,11 +63571,11 @@
       <c r="AB64" s="71"/>
       <c r="AC64" s="71"/>
       <c r="AD64" s="72" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AE64" s="72"/>
       <c r="AF64" s="78" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AG64" s="78"/>
       <c r="AH64" s="78"/>

</xml_diff>